<commit_message>
interrupt vplan collateral after vplan review all items resolved
Signed-off-by: Steve Richmond <Steve.Richmond@silabs.com>
</commit_message>
<xml_diff>
--- a/verif/CV32E40P/VerificationPlan/interrupts/CV32E40P_interrupts.xlsx
+++ b/verif/CV32E40P/VerificationPlan/interrupts/CV32E40P_interrupts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\strichmo\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12AD2640-AA49-41E5-9EC2-FAE96C6A583D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B92CA1-F235-4F94-976E-231E8E42D007}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,12 +35,9 @@
     <author>tc={B5063E1E-F72A-443E-8603-45F80C4143AF}</author>
     <author>tc={0878F7E8-522F-411F-8652-CE9509E3997A}</author>
     <author>tc={8F18CFB5-712B-4251-A5D8-F5CB4694E4E1}</author>
-    <author>tc={C43E46E7-1180-4387-99B5-E69A520849FB}</author>
     <author>tc={BB0B890D-2754-494D-8562-98355052E8A1}</author>
     <author>tc={E4746BD7-7E1B-49BA-8057-92724CF327A0}</author>
-    <author>tc={E6C600D5-65D2-4745-8EE1-8350B73EE880}</author>
     <author>tc={5A201864-4453-4040-AB3A-756259B8674F}</author>
-    <author>tc={2DB420B8-FFC0-42DB-8422-4D3F572BD566}</author>
     <author>tc={DBF72415-992E-4687-89AA-594D06092EF4}</author>
     <author>tc={A5AF476F-84B5-40AF-A1B5-D98D67880192}</author>
     <author>tc={3A65AAB5-516C-486C-93ED-1FA77D4BC523}</author>
@@ -51,7 +48,9 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    The UM actually constrains this to a single clock cycle pulse.  Recommend we update this Feature Decription to match.</t>
+    The UM actually constrains this to a single clock cycle pulse.  Recommend we update this Feature Decription to match.
+Reply:
+    Will constraint this description to a single clock cycle.</t>
       </text>
     </comment>
     <comment ref="F3" authorId="1" shapeId="0" xr:uid="{BC1BB870-6BEF-4BC4-8FD4-3D9CF0E47BCA}">
@@ -59,7 +58,9 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    I would need some more details here.  How can we know the core has "taken" and interrupt?   What does "taken" mean?</t>
+    I would need some more details here.  How can we know the core has "taken" and interrupt?   What does "taken" mean?
+Reply:
+    In both the assertions mentioned in this plan, and in the ISS modeling of the interrupts, irq_ack_o is the signal used as a hint that the core has "taken" and interrupt.  Once this is seen, the assertions will check proper arbitration, enable, etc. and also the ISS will expect the 2nd instruction afterwards to be the first instruction of the winning interrupt (depending on mtvec mode).</t>
       </text>
     </comment>
     <comment ref="D7" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
@@ -69,7 +70,9 @@
 Comment:
     Is this really supported?? Can we ignore?
 Reply:
-    The User Manual clearly documents it and a cursory inspection of the RTL indicates that the core does support it.  A single, dedicated self-checking test should be able to cover this.</t>
+    The User Manual clearly documents it and a cursory inspection of the RTL indicates that the core does support it.  A single, dedicated self-checking test should be able to cover this.
+Reply:
+    Has been addressed in a bootstrap directed test.</t>
       </text>
     </comment>
     <comment ref="F11" authorId="3" shapeId="0" xr:uid="{B5063E1E-F72A-443E-8603-45F80C4143AF}">
@@ -79,7 +82,11 @@
 Comment:
     Why not check against ISS?
 Reply:
-    Agreed, the ISS _should_ be able to support this.</t>
+    Agreed, the ISS _should_ be able to support this.
+Reply:
+    ISS can (and is) checking nested interrupts in the directed interrupt test.  I tried the enable_nested_interrupt in riscv-dv and it is broken (doesn't stack the mepc for example).  Is it necessary to add more random testing for nested interrupts?
+Reply:
+    Went ahead and extended corev-dv to support this.</t>
       </text>
     </comment>
     <comment ref="F12" authorId="4" shapeId="0" xr:uid="{0878F7E8-522F-411F-8652-CE9509E3997A}">
@@ -89,7 +96,11 @@
 Comment:
     Why not check against ISS?
 Reply:
-    Agreed.</t>
+    Agreed.
+Reply:
+    See above.
+Reply:
+    Functionality is checked but in a directed fashion.</t>
       </text>
     </comment>
     <comment ref="F13" authorId="5" shapeId="0" xr:uid="{8F18CFB5-712B-4251-A5D8-F5CB4694E4E1}">
@@ -99,78 +110,70 @@
 Comment:
     Why not check against ISS?
 Reply:
-    Agreed.</t>
+    Agreed.
+Reply:
+    See above.  Functionality is checked but in a directed fashion.
+Reply:
+    Extended corev-dv to support random nested irq handlers.</t>
       </text>
     </comment>
-    <comment ref="D14" authorId="6" shapeId="0" xr:uid="{C43E46E7-1180-4387-99B5-E69A520849FB}">
+    <comment ref="G14" authorId="6" shapeId="0" xr:uid="{BB0B890D-2754-494D-8562-98355052E8A1}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Overkill?  Maybe just check that MSTATUS[MPP] is Read Only. (Already done in CSR DV plan.)</t>
+    Do we need a DSC test for this?  Won't any random test cover this assuming we are checking against the ISS?
+Reply:
+    Yes...just mentioning as a functionality.
+Reply:
+    It should be checked by ISS.</t>
       </text>
     </comment>
-    <comment ref="G15" authorId="7" shapeId="0" xr:uid="{BB0B890D-2754-494D-8562-98355052E8A1}">
+    <comment ref="G21" authorId="7" shapeId="0" xr:uid="{E4746BD7-7E1B-49BA-8057-92724CF327A0}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Do we need a DSC test for this?  Won't any random test cover this assuming we are checking against the ISS?</t>
+    Do we need a DSC test for this?  Won't any random test cover this assuming we are checking against the ISS?
+Reply:
+    Should be covered in random especially with random nested interrupts running now.</t>
       </text>
     </comment>
-    <comment ref="G22" authorId="8" shapeId="0" xr:uid="{E4746BD7-7E1B-49BA-8057-92724CF327A0}">
+    <comment ref="D28" authorId="8" shapeId="0" xr:uid="{5A201864-4453-4040-AB3A-756259B8674F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Do we need a DSC test for this?  Won't any random test cover this assuming we are checking against the ISS?</t>
+    I think the timer is irq_i[7]
+Reply:
+    Thanks...fixing the typo.</t>
       </text>
     </comment>
-    <comment ref="D26" authorId="9" shapeId="0" xr:uid="{E6C600D5-65D2-4745-8EE1-8350B73EE880}">
+    <comment ref="B36" authorId="9" shapeId="0" xr:uid="{DBF72415-992E-4687-89AA-594D06092EF4}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    According to the most current version of the User Manual (0248554b) the Machine Interrupt Pending CSR is Read Only. This is covered in the CSR DV plan, so I recommend we strike this Feture from this DV plan.</t>
+    General comment for all the "Interrupt Instruction" features in this DV plan.  This is important and will produce a large, difficult to fill functional coverage model.  Is there a way to use FV to provide exhaustive coverage of this?
+Reply:
+    Coverage reports show all instructions covered here.
+Reply:
+    Will leave of functional coverage as defined here.</t>
       </text>
     </comment>
-    <comment ref="D30" authorId="10" shapeId="0" xr:uid="{5A201864-4453-4040-AB3A-756259B8674F}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    I think the timer is irq_i[7]</t>
-      </text>
-    </comment>
-    <comment ref="D31" authorId="11" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Determine a reasonable latency maximum.
-Reply:
-    Hmmm.  AFAIK, neither the ISA or UM provide a specification for this.  Therefore, we should not be attempting to verify it.</t>
-      </text>
-    </comment>
-    <comment ref="B39" authorId="12" shapeId="0" xr:uid="{DBF72415-992E-4687-89AA-594D06092EF4}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    General comment for all the "Interrupt Instruction" features in this DV plan.  This is important and will produce a large, difficult to fill functional coverage model.  Is there a way to use FV to provide exhaustive coverage of this?</t>
-      </text>
-    </comment>
-    <comment ref="D76" authorId="13" shapeId="0" xr:uid="{A5AF476F-84B5-40AF-A1B5-D98D67880192}">
+    <comment ref="D71" authorId="10" shapeId="0" xr:uid="{A5AF476F-84B5-40AF-A1B5-D98D67880192}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     This requirement seems untestable for CLINT interrupts.
 Reply:
-    Why is that?</t>
+    Why is that?
+Reply:
+    Will leave as a documented assumption on the interrupt modeling in the verification infrastructure.</t>
       </text>
     </comment>
-    <comment ref="C78" authorId="14" shapeId="0" xr:uid="{3A65AAB5-516C-486C-93ED-1FA77D4BC523}">
+    <comment ref="C73" authorId="11" shapeId="0" xr:uid="{3A65AAB5-516C-486C-93ED-1FA77D4BC523}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -183,7 +186,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="197">
   <si>
     <t>Requirement Location</t>
   </si>
@@ -314,9 +317,6 @@
     <t>Interrupt acknowledge is always a pulse</t>
   </si>
   <si>
-    <t>Interrupt acknowledge is only asserted when a valid interrupt has been taken by the core</t>
-  </si>
-  <si>
     <t>Interrupt acknowledge only asserted once per interrupt</t>
   </si>
   <si>
@@ -488,15 +488,6 @@
     <t>Manipulate MPIE during an ISR and ensure that MSTATUS.MIE reflects this value after MRET instruction</t>
   </si>
   <si>
-    <t>MSTATUS MPP fixed</t>
-  </si>
-  <si>
-    <t>MSTATUS MPP field is always 3 to reflect machine-only mode</t>
-  </si>
-  <si>
-    <t>Ensure that the MSTATUS MPP field is always 3 (for fixed machine mode)</t>
-  </si>
-  <si>
     <t>MIP valid</t>
   </si>
   <si>
@@ -542,31 +533,13 @@
     <t>MIE masking works as expected with all legal combinations of asserted bit</t>
   </si>
   <si>
-    <t>MIP write</t>
-  </si>
-  <si>
-    <t>What does it mean to write to MIP?</t>
-  </si>
-  <si>
     <t>Interrupt arbitration</t>
   </si>
   <si>
     <t>Priority</t>
   </si>
   <si>
-    <t>When multiple interrupts are enabled and pending, the highest-indexed interrupt will always win, with the exception of the timer [11], which is always lowest priority</t>
-  </si>
-  <si>
     <t>Model arbitration in an assertion to ensure priority</t>
-  </si>
-  <si>
-    <t>Pending interrupt starvation</t>
-  </si>
-  <si>
-    <t>When an enabled, pending interrupt is available, the interrupt will be serviced within some reasonable time or cycles (???)</t>
-  </si>
-  <si>
-    <t>When the testbench assumes there is a winning enabled interrupt, ensure the core takes it within a period of cycles, precluding another higher priority trap</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -681,9 +654,6 @@
     <t>MSTATUS[MIE]=0 and MIE=0 after reset.</t>
   </si>
   <si>
-    <t>Greg Additions</t>
-  </si>
-  <si>
     <t>All interrupt lines are level-sensitive.</t>
   </si>
   <si>
@@ -1444,13 +1414,23 @@
       </rPr>
       <t>architecture instructions interrupted</t>
     </r>
+  </si>
+  <si>
+    <t>Interrupt acknowledge is only asserted when a valid interrupt has been taken by the core.
+This acknowledge is used to signal interrupts to the ISS to ensure that the proper MTVEC addressed is entered.</t>
+  </si>
+  <si>
+    <t>When multiple interrupts are enabled and pending, the highest-indexed interrupt will always win, with the exception of the timer [7], which is always lowest priority</t>
+  </si>
+  <si>
+    <t>All assertions and modeling of interrupts for checking assume no edges required to qualify an interrupt.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1496,44 +1476,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="DejaVu Sans"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="DejaVu Sans"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="DejaVu Sans"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="DejaVu Sans"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="DejaVu Sans"/>
       <family val="2"/>
     </font>
@@ -1577,7 +1525,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1613,25 +1561,21 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1724,6 +1668,8 @@
   <person displayName="Mike" id="{CC194F9E-FB21-44BB-955C-76E3AC766B27}" userId="Mike" providerId="None"/>
   <person displayName="Tumbush, Greg" id="{CC2C28E6-F607-4A19-BB77-9C20E40A9306}" userId="Tumbush, Greg" providerId="None"/>
   <person displayName="Steve Richmond" id="{382254AE-A4A6-4C9D-A6B0-229E0C8F1150}" userId="Steve Richmond" providerId="None"/>
+  <person displayName="STEVE RICHMOND" id="{C6893ECA-3FF8-4705-9E6F-D810BC8D0F39}" userId="f2d36e4dc72c5683" providerId="Windows Live"/>
+  <person displayName="Steve Richmond" id="{1DAD76BF-8E72-49CD-A085-4F1A6B6F21DE}" userId="S::strichmo@silabs.com::7ddd8d89-f1b7-4bc9-af01-f5e91b415446" providerId="AD"/>
 </personList>
 </file>
 
@@ -2024,67 +1970,103 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="D2" dT="2020-09-24T12:02:18.12" personId="{CC194F9E-FB21-44BB-955C-76E3AC766B27}" id="{0C500716-74FF-41A9-9E2E-F6AE3084E2A3}">
+  <threadedComment ref="D2" dT="2020-09-24T12:02:18.12" personId="{CC194F9E-FB21-44BB-955C-76E3AC766B27}" id="{0C500716-74FF-41A9-9E2E-F6AE3084E2A3}" done="1">
     <text>The UM actually constrains this to a single clock cycle pulse.  Recommend we update this Feature Decription to match.</text>
   </threadedComment>
-  <threadedComment ref="F3" dT="2020-09-24T12:03:33.36" personId="{CC194F9E-FB21-44BB-955C-76E3AC766B27}" id="{BC1BB870-6BEF-4BC4-8FD4-3D9CF0E47BCA}">
+  <threadedComment ref="D2" dT="2020-09-29T19:57:56.09" personId="{1DAD76BF-8E72-49CD-A085-4F1A6B6F21DE}" id="{5EFA71D8-92CF-46FC-886D-DF0513B32DFA}" parentId="{0C500716-74FF-41A9-9E2E-F6AE3084E2A3}">
+    <text>Will constraint this description to a single clock cycle.</text>
+  </threadedComment>
+  <threadedComment ref="F3" dT="2020-09-24T12:03:33.36" personId="{CC194F9E-FB21-44BB-955C-76E3AC766B27}" id="{BC1BB870-6BEF-4BC4-8FD4-3D9CF0E47BCA}" done="1">
     <text>I would need some more details here.  How can we know the core has "taken" and interrupt?   What does "taken" mean?</text>
   </threadedComment>
-  <threadedComment ref="D7" dT="2020-07-29T20:44:24.78" personId="{382254AE-A4A6-4C9D-A6B0-229E0C8F1150}" id="{3B693C21-E737-4F3F-A7E3-9557F7A71517}">
+  <threadedComment ref="F3" dT="2020-09-27T19:18:22.61" personId="{C6893ECA-3FF8-4705-9E6F-D810BC8D0F39}" id="{6029284C-47EE-4EDC-8341-B123C211E522}" parentId="{BC1BB870-6BEF-4BC4-8FD4-3D9CF0E47BCA}">
+    <text>In both the assertions mentioned in this plan, and in the ISS modeling of the interrupts, irq_ack_o is the signal used as a hint that the core has "taken" and interrupt.  Once this is seen, the assertions will check proper arbitration, enable, etc. and also the ISS will expect the 2nd instruction afterwards to be the first instruction of the winning interrupt (depending on mtvec mode).</text>
+  </threadedComment>
+  <threadedComment ref="D7" dT="2020-07-29T20:44:24.78" personId="{382254AE-A4A6-4C9D-A6B0-229E0C8F1150}" id="{3B693C21-E737-4F3F-A7E3-9557F7A71517}" done="1">
     <text>Is this really supported?? Can we ignore?</text>
   </threadedComment>
   <threadedComment ref="D7" dT="2020-09-24T12:15:42.98" personId="{CC194F9E-FB21-44BB-955C-76E3AC766B27}" id="{608A5E3C-23FE-409E-BB91-0E2510B78FC1}" parentId="{3B693C21-E737-4F3F-A7E3-9557F7A71517}">
     <text>The User Manual clearly documents it and a cursory inspection of the RTL indicates that the core does support it.  A single, dedicated self-checking test should be able to cover this.</text>
   </threadedComment>
-  <threadedComment ref="F11" personId="{CC2C28E6-F607-4A19-BB77-9C20E40A9306}" id="{B5063E1E-F72A-443E-8603-45F80C4143AF}">
+  <threadedComment ref="D7" dT="2020-09-29T19:16:46.52" personId="{C6893ECA-3FF8-4705-9E6F-D810BC8D0F39}" id="{6BFF730C-8CF4-44ED-93BC-32F572335C2A}" parentId="{3B693C21-E737-4F3F-A7E3-9557F7A71517}">
+    <text>Has been addressed in a bootstrap directed test.</text>
+  </threadedComment>
+  <threadedComment ref="F11" personId="{CC2C28E6-F607-4A19-BB77-9C20E40A9306}" id="{B5063E1E-F72A-443E-8603-45F80C4143AF}" done="1">
     <text>Why not check against ISS?</text>
   </threadedComment>
   <threadedComment ref="F11" dT="2020-09-24T12:16:51.28" personId="{CC194F9E-FB21-44BB-955C-76E3AC766B27}" id="{16BD6C78-FC25-4B61-AC52-C57C25AB6894}" parentId="{B5063E1E-F72A-443E-8603-45F80C4143AF}">
     <text>Agreed, the ISS _should_ be able to support this.</text>
   </threadedComment>
-  <threadedComment ref="F12" personId="{CC2C28E6-F607-4A19-BB77-9C20E40A9306}" id="{0878F7E8-522F-411F-8652-CE9509E3997A}">
+  <threadedComment ref="F11" dT="2020-09-27T19:37:59.03" personId="{C6893ECA-3FF8-4705-9E6F-D810BC8D0F39}" id="{05AE9E7F-78D8-48D4-BF8C-82F56C93AD3B}" parentId="{B5063E1E-F72A-443E-8603-45F80C4143AF}">
+    <text>ISS can (and is) checking nested interrupts in the directed interrupt test.  I tried the enable_nested_interrupt in riscv-dv and it is broken (doesn't stack the mepc for example).  Is it necessary to add more random testing for nested interrupts?</text>
+  </threadedComment>
+  <threadedComment ref="F11" dT="2020-09-29T19:17:06.47" personId="{C6893ECA-3FF8-4705-9E6F-D810BC8D0F39}" id="{3E22451B-3EC4-449E-A5FE-9D9C0EE649D2}" parentId="{B5063E1E-F72A-443E-8603-45F80C4143AF}">
+    <text>Went ahead and extended corev-dv to support this.</text>
+  </threadedComment>
+  <threadedComment ref="F12" personId="{CC2C28E6-F607-4A19-BB77-9C20E40A9306}" id="{0878F7E8-522F-411F-8652-CE9509E3997A}" done="1">
     <text>Why not check against ISS?</text>
   </threadedComment>
   <threadedComment ref="F12" dT="2020-09-24T12:21:14.08" personId="{CC194F9E-FB21-44BB-955C-76E3AC766B27}" id="{670573F4-633C-4947-9EA4-A117D7C0DBFF}" parentId="{0878F7E8-522F-411F-8652-CE9509E3997A}">
     <text>Agreed.</text>
   </threadedComment>
-  <threadedComment ref="F13" personId="{CC2C28E6-F607-4A19-BB77-9C20E40A9306}" id="{8F18CFB5-712B-4251-A5D8-F5CB4694E4E1}">
+  <threadedComment ref="F12" dT="2020-09-27T19:38:06.64" personId="{C6893ECA-3FF8-4705-9E6F-D810BC8D0F39}" id="{4FEFCB57-7BDA-40C1-A30A-C5D4060FD44D}" parentId="{0878F7E8-522F-411F-8652-CE9509E3997A}">
+    <text>See above.</text>
+  </threadedComment>
+  <threadedComment ref="F12" dT="2020-09-27T19:38:32.56" personId="{C6893ECA-3FF8-4705-9E6F-D810BC8D0F39}" id="{FAFDC87F-38F1-4D5D-9728-1E6CC0FA86DD}" parentId="{0878F7E8-522F-411F-8652-CE9509E3997A}">
+    <text>Functionality is checked but in a directed fashion.</text>
+  </threadedComment>
+  <threadedComment ref="F13" personId="{CC2C28E6-F607-4A19-BB77-9C20E40A9306}" id="{8F18CFB5-712B-4251-A5D8-F5CB4694E4E1}" done="1">
     <text>Why not check against ISS?</text>
   </threadedComment>
   <threadedComment ref="F13" dT="2020-09-24T12:21:23.11" personId="{CC194F9E-FB21-44BB-955C-76E3AC766B27}" id="{904313C4-66D6-4AB5-9ECD-B5977DDF99AD}" parentId="{8F18CFB5-712B-4251-A5D8-F5CB4694E4E1}">
     <text>Agreed.</text>
   </threadedComment>
-  <threadedComment ref="D14" dT="2020-09-24T12:27:06.05" personId="{CC194F9E-FB21-44BB-955C-76E3AC766B27}" id="{C43E46E7-1180-4387-99B5-E69A520849FB}">
-    <text>Overkill?  Maybe just check that MSTATUS[MPP] is Read Only. (Already done in CSR DV plan.)</text>
+  <threadedComment ref="F13" dT="2020-09-27T19:38:20.75" personId="{C6893ECA-3FF8-4705-9E6F-D810BC8D0F39}" id="{975F08A0-E197-4B0D-B34A-8C33B4B93101}" parentId="{8F18CFB5-712B-4251-A5D8-F5CB4694E4E1}">
+    <text>See above.  Functionality is checked but in a directed fashion.</text>
   </threadedComment>
-  <threadedComment ref="G15" dT="2020-09-24T12:28:31.27" personId="{CC194F9E-FB21-44BB-955C-76E3AC766B27}" id="{BB0B890D-2754-494D-8562-98355052E8A1}">
+  <threadedComment ref="F13" dT="2020-09-29T19:17:22.97" personId="{C6893ECA-3FF8-4705-9E6F-D810BC8D0F39}" id="{DD8157B8-AAB0-4A04-8E46-D4DAF30F4077}" parentId="{8F18CFB5-712B-4251-A5D8-F5CB4694E4E1}">
+    <text>Extended corev-dv to support random nested irq handlers.</text>
+  </threadedComment>
+  <threadedComment ref="G14" dT="2020-09-24T12:28:31.27" personId="{CC194F9E-FB21-44BB-955C-76E3AC766B27}" id="{BB0B890D-2754-494D-8562-98355052E8A1}" done="1">
     <text>Do we need a DSC test for this?  Won't any random test cover this assuming we are checking against the ISS?</text>
   </threadedComment>
-  <threadedComment ref="G22" dT="2020-09-24T12:30:05.13" personId="{CC194F9E-FB21-44BB-955C-76E3AC766B27}" id="{E4746BD7-7E1B-49BA-8057-92724CF327A0}">
+  <threadedComment ref="G14" dT="2020-09-29T01:20:30.23" personId="{C6893ECA-3FF8-4705-9E6F-D810BC8D0F39}" id="{025B2F14-E804-4594-B241-C79A30EDDFA3}" parentId="{BB0B890D-2754-494D-8562-98355052E8A1}">
+    <text>Yes...just mentioning as a functionality.</text>
+  </threadedComment>
+  <threadedComment ref="G14" dT="2020-09-29T19:17:57.88" personId="{C6893ECA-3FF8-4705-9E6F-D810BC8D0F39}" id="{9260653E-EFF2-424F-A781-EA39F3F399CE}" parentId="{BB0B890D-2754-494D-8562-98355052E8A1}">
+    <text>It should be checked by ISS.</text>
+  </threadedComment>
+  <threadedComment ref="G21" dT="2020-09-24T12:30:05.13" personId="{CC194F9E-FB21-44BB-955C-76E3AC766B27}" id="{E4746BD7-7E1B-49BA-8057-92724CF327A0}" done="1">
     <text>Do we need a DSC test for this?  Won't any random test cover this assuming we are checking against the ISS?</text>
   </threadedComment>
-  <threadedComment ref="D26" dT="2020-09-24T12:23:48.32" personId="{CC194F9E-FB21-44BB-955C-76E3AC766B27}" id="{E6C600D5-65D2-4745-8EE1-8350B73EE880}">
-    <text>According to the most current version of the User Manual (0248554b) the Machine Interrupt Pending CSR is Read Only. This is covered in the CSR DV plan, so I recommend we strike this Feture from this DV plan.</text>
+  <threadedComment ref="G21" dT="2020-09-29T01:21:20.91" personId="{C6893ECA-3FF8-4705-9E6F-D810BC8D0F39}" id="{66AF0CC6-5B77-4ED2-A660-669FDAFB34E8}" parentId="{E4746BD7-7E1B-49BA-8057-92724CF327A0}">
+    <text>Should be covered in random especially with random nested interrupts running now.</text>
   </threadedComment>
-  <threadedComment ref="D30" personId="{CC2C28E6-F607-4A19-BB77-9C20E40A9306}" id="{5A201864-4453-4040-AB3A-756259B8674F}">
+  <threadedComment ref="D28" personId="{CC2C28E6-F607-4A19-BB77-9C20E40A9306}" id="{5A201864-4453-4040-AB3A-756259B8674F}" done="1">
     <text>I think the timer is irq_i[7]</text>
   </threadedComment>
-  <threadedComment ref="D31" dT="2020-07-29T23:04:30.12" personId="{382254AE-A4A6-4C9D-A6B0-229E0C8F1150}" id="{2DB420B8-FFC0-42DB-8422-4D3F572BD566}">
-    <text>Determine a reasonable latency maximum.</text>
+  <threadedComment ref="D28" dT="2020-09-27T19:40:32.23" personId="{C6893ECA-3FF8-4705-9E6F-D810BC8D0F39}" id="{9E55D9E6-16C4-484E-93B2-95B7F0CD5065}" parentId="{5A201864-4453-4040-AB3A-756259B8674F}">
+    <text>Thanks...fixing the typo.</text>
   </threadedComment>
-  <threadedComment ref="D31" dT="2020-09-24T12:33:22.49" personId="{CC194F9E-FB21-44BB-955C-76E3AC766B27}" id="{9D4761E7-6C00-4FED-91BF-6446F6E14276}" parentId="{2DB420B8-FFC0-42DB-8422-4D3F572BD566}">
-    <text>Hmmm.  AFAIK, neither the ISA or UM provide a specification for this.  Therefore, we should not be attempting to verify it.</text>
-  </threadedComment>
-  <threadedComment ref="B39" dT="2020-09-24T12:42:19.70" personId="{CC194F9E-FB21-44BB-955C-76E3AC766B27}" id="{DBF72415-992E-4687-89AA-594D06092EF4}">
+  <threadedComment ref="B36" dT="2020-09-24T12:42:19.70" personId="{CC194F9E-FB21-44BB-955C-76E3AC766B27}" id="{DBF72415-992E-4687-89AA-594D06092EF4}" done="1">
     <text>General comment for all the "Interrupt Instruction" features in this DV plan.  This is important and will produce a large, difficult to fill functional coverage model.  Is there a way to use FV to provide exhaustive coverage of this?</text>
   </threadedComment>
-  <threadedComment ref="D76" personId="{CC2C28E6-F607-4A19-BB77-9C20E40A9306}" id="{A5AF476F-84B5-40AF-A1B5-D98D67880192}">
+  <threadedComment ref="B36" dT="2020-09-29T20:07:02.50" personId="{1DAD76BF-8E72-49CD-A085-4F1A6B6F21DE}" id="{B573AD51-FEA3-433F-AA01-34F12FE28222}" parentId="{DBF72415-992E-4687-89AA-594D06092EF4}">
+    <text>Coverage reports show all instructions covered here.</text>
+  </threadedComment>
+  <threadedComment ref="B36" dT="2020-09-29T23:01:29.17" personId="{1DAD76BF-8E72-49CD-A085-4F1A6B6F21DE}" id="{A888FC22-8EC8-46F2-B549-5B794D1A9874}" parentId="{DBF72415-992E-4687-89AA-594D06092EF4}">
+    <text>Will leave of functional coverage as defined here.</text>
+  </threadedComment>
+  <threadedComment ref="D71" personId="{CC2C28E6-F607-4A19-BB77-9C20E40A9306}" id="{A5AF476F-84B5-40AF-A1B5-D98D67880192}" done="1">
     <text>This requirement seems untestable for CLINT interrupts.</text>
   </threadedComment>
-  <threadedComment ref="D76" dT="2020-09-24T12:43:09.85" personId="{CC194F9E-FB21-44BB-955C-76E3AC766B27}" id="{E75BBADE-CFEA-48C0-9C1B-0E9DA9ABA0C3}" parentId="{A5AF476F-84B5-40AF-A1B5-D98D67880192}">
+  <threadedComment ref="D71" dT="2020-09-24T12:43:09.85" personId="{CC194F9E-FB21-44BB-955C-76E3AC766B27}" id="{E75BBADE-CFEA-48C0-9C1B-0E9DA9ABA0C3}" parentId="{A5AF476F-84B5-40AF-A1B5-D98D67880192}">
     <text>Why is that?</text>
   </threadedComment>
-  <threadedComment ref="C78" personId="{CC2C28E6-F607-4A19-BB77-9C20E40A9306}" id="{3A65AAB5-516C-486C-93ED-1FA77D4BC523}">
+  <threadedComment ref="D71" dT="2020-09-29T23:00:54.09" personId="{1DAD76BF-8E72-49CD-A085-4F1A6B6F21DE}" id="{F5208D69-AB1C-4480-BB06-3A6E9F9BC271}" parentId="{A5AF476F-84B5-40AF-A1B5-D98D67880192}">
+    <text>Will leave as a documented assumption on the interrupt modeling in the verification infrastructure.</text>
+  </threadedComment>
+  <threadedComment ref="C73" personId="{CC2C28E6-F607-4A19-BB77-9C20E40A9306}" id="{3A65AAB5-516C-486C-93ED-1FA77D4BC523}" done="1">
     <text>the Pulp tests EM contributed are self-checking.  If an interrupt is serviced properly it should still pass.</text>
   </threadedComment>
 </ThreadedComments>
@@ -2092,19 +2074,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMJ96"/>
+  <dimension ref="A1:AMJ91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="51.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="41.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" style="1" customWidth="1"/>
@@ -2149,10 +2131,10 @@
         <v>35</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>46</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>42</v>
@@ -2171,21 +2153,21 @@
       </c>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:9" s="5" customFormat="1" ht="29.25">
+    <row r="3" spans="1:9" s="5" customFormat="1" ht="72">
       <c r="A3" s="13" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>43</v>
+        <v>194</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>22</v>
@@ -2198,21 +2180,21 @@
       </c>
       <c r="I3" s="6"/>
     </row>
-    <row r="4" spans="1:9" s="5" customFormat="1" ht="43.5">
+    <row r="4" spans="1:9" s="5" customFormat="1" ht="29.25">
       <c r="A4" s="13" t="s">
         <v>35</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>22</v>
@@ -2230,16 +2212,16 @@
         <v>35</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>50</v>
-      </c>
       <c r="E5" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>22</v>
@@ -2257,16 +2239,16 @@
         <v>35</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C6" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="E6" s="7" t="s">
         <v>52</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>53</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>22</v>
@@ -2279,21 +2261,21 @@
       </c>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="1:9" s="5" customFormat="1" ht="30">
+    <row r="7" spans="1:9" s="5" customFormat="1" ht="43.5">
       <c r="A7" s="13" t="s">
         <v>35</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C7" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="E7" s="7" t="s">
         <v>79</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>80</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>10</v>
@@ -2311,16 +2293,16 @@
         <v>35</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="D8" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="E8" s="15" t="s">
         <v>59</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>60</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>16</v>
@@ -2338,16 +2320,16 @@
         <v>35</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>16</v>
@@ -2365,16 +2347,16 @@
         <v>35</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C10" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>64</v>
-      </c>
       <c r="E10" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>16</v>
@@ -2392,22 +2374,22 @@
         <v>35</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C11" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="E11" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>71</v>
-      </c>
       <c r="F11" s="7" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="H11" s="6" t="s">
         <v>12</v>
@@ -2419,22 +2401,22 @@
         <v>35</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C12" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>73</v>
-      </c>
       <c r="E12" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="H12" s="6" t="s">
         <v>15</v>
@@ -2446,76 +2428,76 @@
         <v>35</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C13" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="1:9" s="5" customFormat="1" ht="43.5">
+      <c r="A14" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" s="6"/>
-    </row>
-    <row r="14" spans="1:9" s="5" customFormat="1" ht="29.25">
-      <c r="A14" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>82</v>
-      </c>
       <c r="C14" s="7" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="1:9" s="5" customFormat="1" ht="43.5">
+    <row r="15" spans="1:9" s="5" customFormat="1" ht="29.25">
       <c r="A15" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="H15" s="6" t="s">
         <v>15</v>
@@ -2527,25 +2509,25 @@
         <v>38</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="G16" s="7" t="s">
         <v>23</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I16" s="6"/>
     </row>
@@ -2554,16 +2536,16 @@
         <v>38</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>22</v>
@@ -2576,48 +2558,48 @@
       </c>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="1:9" s="5" customFormat="1" ht="43.5">
+    <row r="18" spans="1:9" s="5" customFormat="1" ht="29.25">
       <c r="A18" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B18" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="1:9" s="5" customFormat="1" ht="29.25">
+      <c r="A19" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I18" s="6"/>
-    </row>
-    <row r="19" spans="1:9" s="5" customFormat="1" ht="43.5">
-      <c r="A19" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>86</v>
-      </c>
       <c r="D19" s="7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>16</v>
@@ -2630,21 +2612,21 @@
       </c>
       <c r="I19" s="6"/>
     </row>
-    <row r="20" spans="1:9" s="5" customFormat="1" ht="29.25">
+    <row r="20" spans="1:9" s="5" customFormat="1" ht="43.5">
       <c r="A20" s="13" t="s">
         <v>35</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>85</v>
+        <v>118</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>16</v>
@@ -2662,16 +2644,16 @@
         <v>35</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>67</v>
+        <v>121</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>68</v>
+        <v>119</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="F21" s="7" t="s">
         <v>16</v>
@@ -2680,7 +2662,7 @@
         <v>23</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I21" s="6"/>
     </row>
@@ -2689,49 +2671,49 @@
         <v>35</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>130</v>
+        <v>149</v>
       </c>
       <c r="F22" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I22" s="6"/>
     </row>
-    <row r="23" spans="1:9" s="5" customFormat="1" ht="43.5">
+    <row r="23" spans="1:9" s="5" customFormat="1" ht="29.25">
       <c r="A23" s="13" t="s">
         <v>35</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>132</v>
+        <v>100</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>133</v>
+        <v>101</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>16</v>
+        <v>102</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>22</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H23" s="6" t="s">
         <v>15</v>
@@ -2743,25 +2725,25 @@
         <v>35</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C24" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="D24" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="E24" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="E24" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="F24" s="18" t="s">
+      <c r="F24" s="7" t="s">
         <v>22</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I24" s="6"/>
     </row>
@@ -2770,16 +2752,16 @@
         <v>35</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C25" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D25" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="E25" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>109</v>
       </c>
       <c r="F25" s="7" t="s">
         <v>22</v>
@@ -2792,73 +2774,81 @@
       </c>
       <c r="I25" s="6"/>
     </row>
-    <row r="26" spans="1:9" s="5" customFormat="1">
+    <row r="26" spans="1:9" s="5" customFormat="1" ht="43.5">
       <c r="A26" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C26" s="16" t="s">
-        <v>119</v>
+        <v>81</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>111</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="6"/>
+        <v>109</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="I26" s="6"/>
     </row>
     <row r="27" spans="1:9" s="5" customFormat="1" ht="29.25">
       <c r="A27" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I27" s="6"/>
+    </row>
+    <row r="28" spans="1:9" s="5" customFormat="1" ht="57.75">
+      <c r="A28" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I27" s="6"/>
-    </row>
-    <row r="28" spans="1:9" s="5" customFormat="1" ht="43.5">
-      <c r="A28" s="13" t="s">
-        <v>38</v>
-      </c>
       <c r="B28" s="7" t="s">
-        <v>82</v>
+        <v>115</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>113</v>
+        <v>195</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="F28" s="7" t="s">
         <v>22</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H28" s="6" t="s">
         <v>18</v>
@@ -2867,46 +2857,46 @@
     </row>
     <row r="29" spans="1:9" s="5" customFormat="1" ht="29.25">
       <c r="A29" s="13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>82</v>
+        <v>127</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I29" s="6"/>
     </row>
-    <row r="30" spans="1:9" s="5" customFormat="1" ht="57.75">
+    <row r="30" spans="1:9" s="5" customFormat="1" ht="29.25">
       <c r="A30" s="13" t="s">
         <v>35</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="F30" s="7" t="s">
         <v>22</v>
@@ -2919,21 +2909,21 @@
       </c>
       <c r="I30" s="6"/>
     </row>
-    <row r="31" spans="1:9" s="5" customFormat="1" ht="57.75">
+    <row r="31" spans="1:9" s="5" customFormat="1" ht="29.25">
       <c r="A31" s="13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="F31" s="7" t="s">
         <v>22</v>
@@ -2951,16 +2941,16 @@
         <v>35</v>
       </c>
       <c r="B32" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C32" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="D32" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="E32" s="7" t="s">
         <v>139</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>140</v>
       </c>
       <c r="F32" s="7" t="s">
         <v>22</v>
@@ -2978,52 +2968,52 @@
         <v>35</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="C33" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D33" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="E33" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E33" s="7" t="s">
-        <v>143</v>
-      </c>
       <c r="F33" s="7" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="G33" s="7" t="s">
         <v>26</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I33" s="6"/>
     </row>
-    <row r="34" spans="1:9" s="5" customFormat="1" ht="29.25">
+    <row r="34" spans="1:9" s="5" customFormat="1" ht="43.5">
       <c r="A34" s="13" t="s">
         <v>35</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="C34" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="D34" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="E34" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="E34" s="7" t="s">
-        <v>146</v>
-      </c>
       <c r="F34" s="7" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I34" s="6"/>
     </row>
@@ -3032,124 +3022,124 @@
         <v>35</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="C35" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="E35" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="D35" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>149</v>
-      </c>
       <c r="F35" s="7" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="G35" s="7" t="s">
         <v>26</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I35" s="6"/>
     </row>
-    <row r="36" spans="1:9" s="5" customFormat="1" ht="43.5">
+    <row r="36" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A36" s="13" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>151</v>
+        <v>125</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>152</v>
+        <v>126</v>
       </c>
       <c r="F36" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H36" s="6" t="s">
         <v>15</v>
       </c>
       <c r="I36" s="6"/>
     </row>
-    <row r="37" spans="1:9" s="5" customFormat="1" ht="43.5">
+    <row r="37" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A37" s="13" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>154</v>
+        <v>125</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>155</v>
+        <v>126</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G37" s="7" t="s">
         <v>23</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I37" s="6"/>
     </row>
-    <row r="38" spans="1:9" s="5" customFormat="1" ht="29.25">
+    <row r="38" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A38" s="13" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>156</v>
+        <v>125</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>157</v>
+        <v>126</v>
       </c>
       <c r="F38" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H38" s="6" t="s">
         <v>15</v>
       </c>
       <c r="I38" s="6"/>
     </row>
-    <row r="39" spans="1:9" s="5" customFormat="1" ht="58.5">
+    <row r="39" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A39" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F39" s="7" t="s">
         <v>16</v>
@@ -3162,21 +3152,21 @@
       </c>
       <c r="I39" s="6"/>
     </row>
-    <row r="40" spans="1:9" s="5" customFormat="1" ht="58.5">
+    <row r="40" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A40" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F40" s="7" t="s">
         <v>16</v>
@@ -3189,21 +3179,21 @@
       </c>
       <c r="I40" s="6"/>
     </row>
-    <row r="41" spans="1:9" s="5" customFormat="1" ht="58.5">
+    <row r="41" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A41" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F41" s="7" t="s">
         <v>16</v>
@@ -3216,21 +3206,21 @@
       </c>
       <c r="I41" s="6"/>
     </row>
-    <row r="42" spans="1:9" s="5" customFormat="1" ht="58.5">
+    <row r="42" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A42" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F42" s="7" t="s">
         <v>16</v>
@@ -3243,21 +3233,21 @@
       </c>
       <c r="I42" s="6"/>
     </row>
-    <row r="43" spans="1:9" s="5" customFormat="1" ht="58.5">
+    <row r="43" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A43" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F43" s="7" t="s">
         <v>16</v>
@@ -3270,21 +3260,21 @@
       </c>
       <c r="I43" s="6"/>
     </row>
-    <row r="44" spans="1:9" s="5" customFormat="1" ht="58.5">
+    <row r="44" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A44" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>177</v>
+        <v>124</v>
+      </c>
+      <c r="C44" s="20" t="s">
+        <v>170</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F44" s="7" t="s">
         <v>16</v>
@@ -3297,21 +3287,21 @@
       </c>
       <c r="I44" s="6"/>
     </row>
-    <row r="45" spans="1:9" s="5" customFormat="1" ht="58.5">
+    <row r="45" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A45" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>178</v>
+        <v>124</v>
+      </c>
+      <c r="C45" s="20" t="s">
+        <v>169</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F45" s="7" t="s">
         <v>16</v>
@@ -3324,21 +3314,21 @@
       </c>
       <c r="I45" s="6"/>
     </row>
-    <row r="46" spans="1:9" s="5" customFormat="1" ht="58.5">
+    <row r="46" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A46" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>179</v>
+        <v>124</v>
+      </c>
+      <c r="C46" s="20" t="s">
+        <v>171</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F46" s="7" t="s">
         <v>16</v>
@@ -3351,21 +3341,21 @@
       </c>
       <c r="I46" s="6"/>
     </row>
-    <row r="47" spans="1:9" s="5" customFormat="1" ht="59.25">
+    <row r="47" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A47" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C47" s="24" t="s">
-        <v>181</v>
+        <v>124</v>
+      </c>
+      <c r="C47" s="20" t="s">
+        <v>172</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F47" s="7" t="s">
         <v>16</v>
@@ -3383,16 +3373,16 @@
         <v>38</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C48" s="24" t="s">
-        <v>180</v>
+        <v>124</v>
+      </c>
+      <c r="C48" s="20" t="s">
+        <v>173</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F48" s="7" t="s">
         <v>16</v>
@@ -3405,21 +3395,21 @@
       </c>
       <c r="I48" s="6"/>
     </row>
-    <row r="49" spans="1:9" s="5" customFormat="1" ht="59.25">
+    <row r="49" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A49" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C49" s="24" t="s">
-        <v>182</v>
+        <v>124</v>
+      </c>
+      <c r="C49" s="20" t="s">
+        <v>174</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F49" s="7" t="s">
         <v>16</v>
@@ -3437,16 +3427,16 @@
         <v>38</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C50" s="24" t="s">
-        <v>183</v>
+        <v>124</v>
+      </c>
+      <c r="C50" s="20" t="s">
+        <v>175</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F50" s="7" t="s">
         <v>16</v>
@@ -3459,21 +3449,21 @@
       </c>
       <c r="I50" s="6"/>
     </row>
-    <row r="51" spans="1:9" s="5" customFormat="1" ht="59.25">
+    <row r="51" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A51" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C51" s="24" t="s">
-        <v>184</v>
+        <v>124</v>
+      </c>
+      <c r="C51" s="20" t="s">
+        <v>176</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F51" s="7" t="s">
         <v>16</v>
@@ -3491,16 +3481,16 @@
         <v>38</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C52" s="24" t="s">
-        <v>185</v>
+        <v>124</v>
+      </c>
+      <c r="C52" s="20" t="s">
+        <v>177</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F52" s="7" t="s">
         <v>16</v>
@@ -3513,21 +3503,21 @@
       </c>
       <c r="I52" s="6"/>
     </row>
-    <row r="53" spans="1:9" s="5" customFormat="1" ht="59.25">
+    <row r="53" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A53" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C53" s="24" t="s">
-        <v>186</v>
+        <v>124</v>
+      </c>
+      <c r="C53" s="20" t="s">
+        <v>178</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F53" s="7" t="s">
         <v>16</v>
@@ -3545,16 +3535,16 @@
         <v>38</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C54" s="24" t="s">
-        <v>187</v>
+        <v>124</v>
+      </c>
+      <c r="C54" s="20" t="s">
+        <v>179</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F54" s="7" t="s">
         <v>16</v>
@@ -3567,21 +3557,21 @@
       </c>
       <c r="I54" s="6"/>
     </row>
-    <row r="55" spans="1:9" s="5" customFormat="1" ht="59.25">
+    <row r="55" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A55" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C55" s="24" t="s">
-        <v>188</v>
+        <v>124</v>
+      </c>
+      <c r="C55" s="20" t="s">
+        <v>180</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F55" s="7" t="s">
         <v>16</v>
@@ -3599,16 +3589,16 @@
         <v>38</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C56" s="24" t="s">
-        <v>189</v>
+        <v>124</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>181</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F56" s="7" t="s">
         <v>16</v>
@@ -3621,21 +3611,21 @@
       </c>
       <c r="I56" s="6"/>
     </row>
-    <row r="57" spans="1:9" s="5" customFormat="1" ht="59.25">
+    <row r="57" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A57" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C57" s="24" t="s">
-        <v>190</v>
+        <v>124</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>182</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F57" s="7" t="s">
         <v>16</v>
@@ -3648,21 +3638,21 @@
       </c>
       <c r="I57" s="6"/>
     </row>
-    <row r="58" spans="1:9" s="5" customFormat="1" ht="59.25">
+    <row r="58" spans="1:9" s="5" customFormat="1" ht="45">
       <c r="A58" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C58" s="24" t="s">
-        <v>191</v>
+        <v>124</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>183</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F58" s="7" t="s">
         <v>16</v>
@@ -3675,21 +3665,21 @@
       </c>
       <c r="I58" s="6"/>
     </row>
-    <row r="59" spans="1:9" s="5" customFormat="1" ht="58.5">
+    <row r="59" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A59" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F59" s="7" t="s">
         <v>16</v>
@@ -3702,21 +3692,21 @@
       </c>
       <c r="I59" s="6"/>
     </row>
-    <row r="60" spans="1:9" s="5" customFormat="1" ht="44.25">
+    <row r="60" spans="1:9" s="5" customFormat="1" ht="59.25">
       <c r="A60" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F60" s="7" t="s">
         <v>16</v>
@@ -3729,21 +3719,21 @@
       </c>
       <c r="I60" s="6"/>
     </row>
-    <row r="61" spans="1:9" s="5" customFormat="1" ht="60">
+    <row r="61" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A61" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F61" s="7" t="s">
         <v>16</v>
@@ -3756,21 +3746,21 @@
       </c>
       <c r="I61" s="6"/>
     </row>
-    <row r="62" spans="1:9" s="5" customFormat="1" ht="59.25">
+    <row r="62" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A62" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F62" s="7" t="s">
         <v>16</v>
@@ -3783,21 +3773,21 @@
       </c>
       <c r="I62" s="6"/>
     </row>
-    <row r="63" spans="1:9" s="5" customFormat="1" ht="59.25">
+    <row r="63" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A63" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F63" s="7" t="s">
         <v>16</v>
@@ -3810,21 +3800,21 @@
       </c>
       <c r="I63" s="6"/>
     </row>
-    <row r="64" spans="1:9" s="5" customFormat="1" ht="59.25">
+    <row r="64" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A64" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C64" s="7" t="s">
-        <v>197</v>
+        <v>124</v>
+      </c>
+      <c r="C64" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E64" s="7" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F64" s="7" t="s">
         <v>16</v>
@@ -3837,21 +3827,21 @@
       </c>
       <c r="I64" s="6"/>
     </row>
-    <row r="65" spans="1:9" s="5" customFormat="1" ht="59.25">
+    <row r="65" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A65" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C65" s="7" t="s">
-        <v>198</v>
+        <v>124</v>
+      </c>
+      <c r="C65" s="20" t="s">
+        <v>190</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F65" s="7" t="s">
         <v>16</v>
@@ -3864,21 +3854,21 @@
       </c>
       <c r="I65" s="6"/>
     </row>
-    <row r="66" spans="1:9" s="5" customFormat="1" ht="59.25">
+    <row r="66" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A66" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C66" s="7" t="s">
-        <v>199</v>
+        <v>124</v>
+      </c>
+      <c r="C66" s="20" t="s">
+        <v>191</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F66" s="7" t="s">
         <v>16</v>
@@ -3891,21 +3881,21 @@
       </c>
       <c r="I66" s="6"/>
     </row>
-    <row r="67" spans="1:9" s="5" customFormat="1" ht="59.25">
+    <row r="67" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A67" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C67" s="24" t="s">
-        <v>200</v>
+        <v>124</v>
+      </c>
+      <c r="C67" s="20" t="s">
+        <v>192</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F67" s="7" t="s">
         <v>16</v>
@@ -3918,21 +3908,21 @@
       </c>
       <c r="I67" s="6"/>
     </row>
-    <row r="68" spans="1:9" s="5" customFormat="1" ht="59.25">
+    <row r="68" spans="1:9" s="5" customFormat="1" ht="58.5">
       <c r="A68" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C68" s="24" t="s">
-        <v>201</v>
+        <v>124</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>193</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F68" s="7" t="s">
         <v>16</v>
@@ -3945,236 +3935,194 @@
       </c>
       <c r="I68" s="6"/>
     </row>
-    <row r="69" spans="1:9" s="5" customFormat="1" ht="59.25">
+    <row r="69" spans="1:9" s="5" customFormat="1" ht="29.25">
       <c r="A69" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="D69" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="E69" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="F69" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G69" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H69" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I69" s="6"/>
+    </row>
+    <row r="70" spans="1:9" s="5" customFormat="1" ht="29.25">
+      <c r="A70" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="D70" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="E70" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="F70" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G70" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H70" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I70" s="6"/>
+    </row>
+    <row r="71" spans="1:9" s="5" customFormat="1" ht="43.5">
+      <c r="A71" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B71" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="D71" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="E71" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="F71" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G71" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H71" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I71" s="6"/>
+    </row>
+    <row r="72" spans="1:9" s="5" customFormat="1" ht="29.25">
+      <c r="A72" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D72" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="E72" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="F72" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G72" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H72" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I72" s="6"/>
+    </row>
+    <row r="73" spans="1:9" s="5" customFormat="1" ht="43.5">
+      <c r="A73" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B69" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C69" s="24" t="s">
-        <v>202</v>
-      </c>
-      <c r="D69" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="E69" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="F69" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G69" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H69" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I69" s="6"/>
-    </row>
-    <row r="70" spans="1:9" s="5" customFormat="1" ht="59.25">
-      <c r="A70" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B70" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C70" s="24" t="s">
-        <v>203</v>
-      </c>
-      <c r="D70" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="E70" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="F70" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G70" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H70" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I70" s="6"/>
-    </row>
-    <row r="71" spans="1:9" s="5" customFormat="1" ht="58.5">
-      <c r="A71" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B71" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C71" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="D71" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="E71" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="F71" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G71" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H71" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I71" s="6"/>
-    </row>
-    <row r="72" spans="1:9" s="5" customFormat="1">
-      <c r="A72" s="13"/>
-      <c r="B72" s="7"/>
-      <c r="C72" s="7"/>
-      <c r="D72" s="7"/>
-      <c r="E72" s="7"/>
-      <c r="F72" s="7"/>
-      <c r="G72" s="7"/>
-      <c r="H72" s="6"/>
-      <c r="I72" s="6"/>
-    </row>
-    <row r="73" spans="1:9" s="5" customFormat="1">
-      <c r="A73" s="22" t="s">
-        <v>165</v>
-      </c>
-      <c r="B73" s="7"/>
-      <c r="C73" s="7"/>
-      <c r="D73" s="7"/>
-      <c r="E73" s="7"/>
-      <c r="F73" s="7"/>
-      <c r="G73" s="7"/>
-      <c r="H73" s="6"/>
+      <c r="B73" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="F73" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G73" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H73" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="I73" s="6"/>
     </row>
-    <row r="74" spans="1:9" s="5" customFormat="1" ht="29.25">
-      <c r="A74" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B74" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C74" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="D74" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="E74" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="F74" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G74" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H74" s="6" t="s">
-        <v>15</v>
-      </c>
+    <row r="74" spans="1:9" s="5" customFormat="1">
+      <c r="A74" s="6"/>
+      <c r="B74" s="7"/>
+      <c r="C74" s="7"/>
+      <c r="D74" s="7"/>
+      <c r="E74" s="7"/>
+      <c r="F74" s="7"/>
+      <c r="G74" s="7"/>
+      <c r="H74" s="6"/>
       <c r="I74" s="6"/>
     </row>
-    <row r="75" spans="1:9" s="5" customFormat="1" ht="29.25">
-      <c r="A75" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B75" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C75" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="D75" s="19" t="s">
-        <v>162</v>
-      </c>
-      <c r="E75" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F75" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G75" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H75" s="6" t="s">
-        <v>15</v>
-      </c>
+    <row r="75" spans="1:9" s="5" customFormat="1">
+      <c r="A75" s="6"/>
+      <c r="B75" s="7"/>
+      <c r="C75" s="7"/>
+      <c r="D75" s="7"/>
+      <c r="E75" s="7"/>
+      <c r="F75" s="7"/>
+      <c r="G75" s="7"/>
+      <c r="H75" s="6"/>
       <c r="I75" s="6"/>
     </row>
-    <row r="76" spans="1:9" s="5" customFormat="1" ht="29.25">
-      <c r="A76" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B76" s="20" t="s">
-        <v>167</v>
-      </c>
-      <c r="C76" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="D76" s="19" t="s">
-        <v>166</v>
-      </c>
+    <row r="76" spans="1:9" s="5" customFormat="1">
+      <c r="A76" s="6"/>
+      <c r="B76" s="7"/>
+      <c r="C76" s="7"/>
+      <c r="D76" s="7"/>
       <c r="E76" s="7"/>
       <c r="F76" s="7"/>
       <c r="G76" s="7"/>
       <c r="H76" s="6"/>
       <c r="I76" s="6"/>
     </row>
-    <row r="77" spans="1:9" s="5" customFormat="1" ht="29.25">
-      <c r="A77" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C77" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D77" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E77" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="F77" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G77" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H77" s="6" t="s">
-        <v>15</v>
-      </c>
+    <row r="77" spans="1:9" s="5" customFormat="1">
+      <c r="A77" s="6"/>
+      <c r="B77" s="7"/>
+      <c r="C77" s="7"/>
+      <c r="D77" s="7"/>
+      <c r="E77" s="7"/>
+      <c r="F77" s="7"/>
+      <c r="G77" s="7"/>
+      <c r="H77" s="6"/>
       <c r="I77" s="6"/>
     </row>
-    <row r="78" spans="1:9" s="5" customFormat="1" ht="57.75">
-      <c r="A78" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B78" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C78" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="D78" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="E78" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="F78" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G78" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H78" s="6" t="s">
-        <v>15</v>
-      </c>
+    <row r="78" spans="1:9" s="5" customFormat="1">
+      <c r="A78" s="6"/>
+      <c r="B78" s="7"/>
+      <c r="C78" s="7"/>
+      <c r="D78" s="7"/>
+      <c r="E78" s="7"/>
+      <c r="F78" s="7"/>
+      <c r="G78" s="7"/>
+      <c r="H78" s="6"/>
       <c r="I78" s="6"/>
     </row>
     <row r="79" spans="1:9" s="5" customFormat="1">
@@ -4309,77 +4257,22 @@
       <c r="H90" s="6"/>
       <c r="I90" s="6"/>
     </row>
-    <row r="91" spans="1:9" s="5" customFormat="1">
-      <c r="A91" s="6"/>
-      <c r="B91" s="7"/>
-      <c r="C91" s="7"/>
-      <c r="D91" s="7"/>
-      <c r="E91" s="7"/>
-      <c r="F91" s="7"/>
-      <c r="G91" s="7"/>
-      <c r="H91" s="6"/>
-      <c r="I91" s="6"/>
-    </row>
-    <row r="92" spans="1:9" s="5" customFormat="1">
-      <c r="A92" s="6"/>
-      <c r="B92" s="7"/>
-      <c r="C92" s="7"/>
-      <c r="D92" s="7"/>
-      <c r="E92" s="7"/>
-      <c r="F92" s="7"/>
-      <c r="G92" s="7"/>
-      <c r="H92" s="6"/>
-      <c r="I92" s="6"/>
-    </row>
-    <row r="93" spans="1:9" s="5" customFormat="1">
-      <c r="A93" s="6"/>
-      <c r="B93" s="7"/>
-      <c r="C93" s="7"/>
-      <c r="D93" s="7"/>
-      <c r="E93" s="7"/>
-      <c r="F93" s="7"/>
-      <c r="G93" s="7"/>
-      <c r="H93" s="6"/>
-      <c r="I93" s="6"/>
-    </row>
-    <row r="94" spans="1:9" s="5" customFormat="1">
-      <c r="A94" s="6"/>
-      <c r="B94" s="7"/>
-      <c r="C94" s="7"/>
-      <c r="D94" s="7"/>
-      <c r="E94" s="7"/>
-      <c r="F94" s="7"/>
-      <c r="G94" s="7"/>
-      <c r="H94" s="6"/>
-      <c r="I94" s="6"/>
-    </row>
-    <row r="95" spans="1:9" s="5" customFormat="1">
-      <c r="A95" s="6"/>
-      <c r="B95" s="7"/>
-      <c r="C95" s="7"/>
-      <c r="D95" s="7"/>
-      <c r="E95" s="7"/>
-      <c r="F95" s="7"/>
-      <c r="G95" s="7"/>
-      <c r="H95" s="6"/>
-      <c r="I95" s="6"/>
-    </row>
-    <row r="96" spans="1:9" s="8" customFormat="1">
-      <c r="A96" s="23" t="s">
+    <row r="91" spans="1:9" s="8" customFormat="1">
+      <c r="A91" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B96" s="23"/>
-      <c r="C96" s="23"/>
-      <c r="D96" s="23"/>
-      <c r="E96" s="23"/>
-      <c r="F96" s="23"/>
-      <c r="G96" s="23"/>
-      <c r="H96" s="23"/>
-      <c r="I96" s="23"/>
+      <c r="B91" s="21"/>
+      <c r="C91" s="21"/>
+      <c r="D91" s="21"/>
+      <c r="E91" s="21"/>
+      <c r="F91" s="21"/>
+      <c r="G91" s="21"/>
+      <c r="H91" s="21"/>
+      <c r="I91" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A96:I96"/>
+    <mergeCell ref="A91:I91"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4394,7 +4287,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>H2:H95</xm:sqref>
+          <xm:sqref>H2:H90</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
@@ -4403,7 +4296,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>G2:G95</xm:sqref>
+          <xm:sqref>G2:G90</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
@@ -4412,7 +4305,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>F2:F95</xm:sqref>
+          <xm:sqref>F2:F90</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4595,7 +4488,7 @@
         <v>39</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="2:5">

</xml_diff>